<commit_message>
Atualização das planilhas de backlog e riscos
</commit_message>
<xml_diff>
--- a/Projeto-Documentacao/Planilhas/Backlog.xlsx
+++ b/Projeto-Documentacao/Planilhas/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\REGINALDO\Documents\Curso do Romão\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\grupo3-sa\Projeto-Documentacao\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67555C6A-8682-4190-8378-DCD99640FD47}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFAC96B-61A5-481D-8454-3DC3D9C4BC63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{84BC08A5-9824-475D-BDF3-0EAC86DFDB14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{84BC08A5-9824-475D-BDF3-0EAC86DFDB14}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,6 @@
     <t>Site Institucional.</t>
   </si>
   <si>
-    <t>Tela de Cadastro.</t>
-  </si>
-  <si>
-    <t>Tela de Login.</t>
-  </si>
-  <si>
     <t>Graficos.</t>
   </si>
   <si>
@@ -64,6 +58,12 @@
   </si>
   <si>
     <t>Sensor.</t>
+  </si>
+  <si>
+    <t>Tela de login</t>
+  </si>
+  <si>
+    <t>Tela de cadastro</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,10 +508,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,10 +519,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -552,7 +552,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>

</xml_diff>